<commit_message>
Journal de travai - Héléna
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Helena.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Helena.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -36,19 +36,22 @@
     <t>Journal de travail</t>
   </si>
   <si>
-    <t>Albert Einstein</t>
-  </si>
-  <si>
-    <t>blablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablabla</t>
-  </si>
-  <si>
-    <t>blablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablabla</t>
+    <t>Héléna Reymond</t>
+  </si>
+  <si>
+    <t>Recherche d'idée de fonctionnalités pour l'application de budget (analyse d'applications existantes, réflexions personnelles)</t>
+  </si>
+  <si>
+    <t>Co-rédaction, correction et relecture du cahier des charges réalisé par Daniel</t>
+  </si>
+  <si>
+    <t>Recherche d'idées de projets en classe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -164,8 +167,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{8BF2A1D9-2379-45F5-94F9-3165E560B691}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -439,11 +470,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,32 +507,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>43150</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>43151</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>43152</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>43151</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
@@ -629,7 +666,7 @@
       </c>
       <c r="C32" s="9">
         <f>SUM(C5:C31)</f>
-        <v>3</v>
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal de travail Héléna
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Helena.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Helena.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FA9018-BC29-40BA-95D8-96E969212A48}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -42,10 +43,49 @@
     <t>Recherche d'idée de fonctionnalités pour l'application de budget (analyse d'applications existantes, réflexions personnelles)</t>
   </si>
   <si>
-    <t>Co-rédaction, correction et relecture du cahier des charges réalisé par Daniel</t>
-  </si>
-  <si>
     <t>Recherche d'idées de projets en classe</t>
+  </si>
+  <si>
+    <t>Rédaction et recherche de fonctionnalités pour le cahier des charges</t>
+  </si>
+  <si>
+    <t>Discussion autour des fonctionnalités</t>
+  </si>
+  <si>
+    <t>Relecture, correction des fonctionnalités pour la cahier des charges</t>
+  </si>
+  <si>
+    <t>Co-rédaction, correction et relecture de la proposition de projet réalisée par Daniel</t>
+  </si>
+  <si>
+    <t>Débat sur la proposition de projet avec l'enseignant</t>
+  </si>
+  <si>
+    <t>Ecriture du cahier des charges</t>
+  </si>
+  <si>
+    <t>Finalisation du cahier des charges, du Gantt et de la répartition des heures</t>
+  </si>
+  <si>
+    <t>Réunion de groupe pour les dernières discussions autour du cahier des charges</t>
+  </si>
+  <si>
+    <t>Discussion et réflexion pour la création du schéma relationnel</t>
+  </si>
+  <si>
+    <t>Réalisation du schéma relationnel</t>
+  </si>
+  <si>
+    <t>Création et test du script de création de la base de données</t>
+  </si>
+  <si>
+    <t>Réunion de groupe pour dernière validation du schéma relationnel, des maquettes et du schéma UML (14h45-16h)</t>
+  </si>
+  <si>
+    <t>Mise à jour / correction du schéma relationnel (16h-16h30)</t>
+  </si>
+  <si>
+    <t>Mise à jour du script de base de données (contraintes d'unicité, changement de noms de table, contraintes de mises à jour)</t>
   </si>
 </sst>
 </file>
@@ -141,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -160,8 +200,26 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,10 +546,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
@@ -512,10 +570,10 @@
         <v>43150</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="8">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -534,76 +592,154 @@
         <v>43151</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
+      <c r="A8" s="10">
+        <v>43157</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>43158</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
+      <c r="A10" s="10">
+        <v>43159</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>43162</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>43163</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="12">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
+      <c r="A13" s="10">
+        <v>43163</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>43164</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="3">
+        <v>43170</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="3">
+        <v>43170</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="8"/>
+      <c r="A17" s="14">
+        <v>43177</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>43178</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="8"/>
+      <c r="A19" s="10">
+        <v>43178</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>43184</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
@@ -661,12 +797,17 @@
       <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="9">
-        <f>SUM(C5:C31)</f>
-        <v>1.25</v>
+      <c r="C33" s="9">
+        <f>SUM(C5:C32)</f>
+        <v>18.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal de travail - Héléna
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Helena.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Helena.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FA9018-BC29-40BA-95D8-96E969212A48}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65EE85B-04FD-46EF-8A5C-A7BA4BDAC14B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Héléna Reymond</t>
   </si>
   <si>
-    <t>Recherche d'idée de fonctionnalités pour l'application de budget (analyse d'applications existantes, réflexions personnelles)</t>
-  </si>
-  <si>
     <t>Recherche d'idées de projets en classe</t>
   </si>
   <si>
@@ -55,37 +52,122 @@
     <t>Relecture, correction des fonctionnalités pour la cahier des charges</t>
   </si>
   <si>
-    <t>Co-rédaction, correction et relecture de la proposition de projet réalisée par Daniel</t>
-  </si>
-  <si>
     <t>Débat sur la proposition de projet avec l'enseignant</t>
   </si>
   <si>
-    <t>Ecriture du cahier des charges</t>
-  </si>
-  <si>
     <t>Finalisation du cahier des charges, du Gantt et de la répartition des heures</t>
   </si>
   <si>
-    <t>Réunion de groupe pour les dernières discussions autour du cahier des charges</t>
-  </si>
-  <si>
-    <t>Discussion et réflexion pour la création du schéma relationnel</t>
-  </si>
-  <si>
-    <t>Réalisation du schéma relationnel</t>
-  </si>
-  <si>
     <t>Création et test du script de création de la base de données</t>
   </si>
   <si>
-    <t>Réunion de groupe pour dernière validation du schéma relationnel, des maquettes et du schéma UML (14h45-16h)</t>
-  </si>
-  <si>
-    <t>Mise à jour / correction du schéma relationnel (16h-16h30)</t>
-  </si>
-  <si>
-    <t>Mise à jour du script de base de données (contraintes d'unicité, changement de noms de table, contraintes de mises à jour)</t>
+    <t>Ecriture des fichiers de création de base de données Postgres et Derby selon le script SQL créé</t>
+  </si>
+  <si>
+    <t>Ecriture du fichier de création des triggers et procédures, et tests</t>
+  </si>
+  <si>
+    <t>Ecriture du rapport</t>
+  </si>
+  <si>
+    <t>Intégration du rapport modifié de François
+Coordination du groupe pour faire fonctionner l'enregistrement et connexion de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Réunion de groupe pour la mise en place de la base de données sur une solution d'hébergement
+Création des procédures stockées</t>
+  </si>
+  <si>
+    <t>Modification du fichier DALClientMapper
+Ecriture du fichier DALBankAccountMapper
+Ecriture du fichier DALCategoryMapper
+Ecriture du fichier DALDebtMapper</t>
+  </si>
+  <si>
+    <t>Recherche d'idée de fonctionnalités pour l'application de budget (analyse d'applications existantes, réflexions personnelles)
+Co-rédaction, correction et relecture de la proposition de projet réalisée par Daniel</t>
+  </si>
+  <si>
+    <t>Réunion de groupe pour les dernières discussions autour du cahier des charges
+Ecriture du cahier des charges</t>
+  </si>
+  <si>
+    <t>Discussion et réflexion pour la création du schéma relationnel
+Réalisation du schéma relationnel</t>
+  </si>
+  <si>
+    <t>Réunion de groupe pour dernière validation du schéma relationnel, des maquettes et du schéma UML
+Mise à jour / correction du schéma relationnel</t>
+  </si>
+  <si>
+    <t>Mise à jour du script de base de données (contraintes d'unicité, changement de noms de table, contraintes de mises à jour)
+Etablissement des mécanismes des différentes procédures/triggers</t>
+  </si>
+  <si>
+    <t>Réunion du groupe DB pour discussion autour des scripts SQL, PostgreSQL, SQLite, Hibernate</t>
+  </si>
+  <si>
+    <t>Correction/complétion du powerpoint
+Présentation de l'avancement du projet
+Réunion avec Guillaume pour apprentissage rapide d'Hibernate</t>
+  </si>
+  <si>
+    <t>Intégration des rapports de Bryan et Guillaume</t>
+  </si>
+  <si>
+    <t>Intégration des rapports de François et Bryan
+Résolution de problèmes au niveau de la DAL avec Guillaume</t>
+  </si>
+  <si>
+    <t>Intégration des rapports de François et de Bryan
+Nettoyage du fichier DALClientMapper
+Ecriture du fichier DALBankAccountMapper</t>
+  </si>
+  <si>
+    <t>Ecriture du fichier DALRecurrenceMapper
+Nettoyage du journal de travail</t>
+  </si>
+  <si>
+    <t>Semaine 1</t>
+  </si>
+  <si>
+    <t>Total des heures par semaine</t>
+  </si>
+  <si>
+    <t>Semaine 2</t>
+  </si>
+  <si>
+    <t>Semaine 3</t>
+  </si>
+  <si>
+    <t>Semaine 4</t>
+  </si>
+  <si>
+    <t>Semaine 5</t>
+  </si>
+  <si>
+    <t>Semaine 6</t>
+  </si>
+  <si>
+    <t>Semaine 7</t>
+  </si>
+  <si>
+    <t>Semaine 8</t>
+  </si>
+  <si>
+    <t>Semaine 9</t>
+  </si>
+  <si>
+    <t>Semaine 10</t>
+  </si>
+  <si>
+    <t>Semaine 11</t>
+  </si>
+  <si>
+    <t>Semaine 12</t>
+  </si>
+  <si>
+    <t>Semaine 13</t>
   </si>
 </sst>
 </file>
@@ -154,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -177,11 +259,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -209,9 +302,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -220,6 +310,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,10 +642,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
@@ -570,244 +666,464 @@
         <v>43150</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>43151</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>43157</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>43151</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
-        <v>43157</v>
+        <v>43158</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
-        <v>43158</v>
+        <v>43159</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
-        <v>43159</v>
+        <v>43162</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="12">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
-        <v>43162</v>
+        <v>43163</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C11" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>43164</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>43170</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>43177</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <v>43178</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>43184</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="15">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
-        <v>43163</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="12">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
-        <v>43163</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="12">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>43164</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="8">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>43170</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>43170</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>43185</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
-        <v>43177</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="16">
-        <v>0.5</v>
+      <c r="C17" s="12">
+        <v>1.25</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
-        <v>43178</v>
+        <v>43187</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C18" s="12">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
-        <v>43178</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="13">
+        <v>43194</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
-        <v>43184</v>
+        <v>43199</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C20" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="8"/>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>43201</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="10">
+        <v>43202</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="8"/>
+      <c r="A23" s="10">
+        <v>43204</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13">
+        <v>43206</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="15">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="13">
+        <v>43207</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="15">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="8"/>
+      <c r="A26" s="13">
+        <v>43209</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <v>43213</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="8"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="5" t="s">
+      <c r="A28" s="10">
+        <v>43218</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="12">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>43219</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="12">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
+        <v>43220</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="15">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="13">
+        <v>43191</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="13">
+        <v>43192</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="9">
-        <f>SUM(C5:C32)</f>
-        <v>18.25</v>
+      <c r="C37" s="9">
+        <f>SUM(C5:C36)</f>
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="8">
+        <f>SUM(C5:C6)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="8">
+        <f>SUM(C7:C11)</f>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="8">
+        <f>SUM(C12:C13)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="8">
+        <f>SUM(C14)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="8">
+        <f>SUM(C15:C16)</f>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="8">
+        <f>SUM(C17:C18)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="8">
+        <f>SUM(C19)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="8">
+        <f>SUM(C20:C23)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="8">
+        <f>SUM(C24:C26)</f>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="8">
+        <f>SUM(C27:C29)</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="8">
+        <f>SUM(C30:C32)</f>
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="9">
+        <f>SUM(C41:C53)</f>
+        <v>49.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>